<commit_message>
cambios mensuales`, nuevas estimaciones recuperados
</commit_message>
<xml_diff>
--- a/ccaa_semanal_14_7.xlsx
+++ b/ccaa_semanal_14_7.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2741" uniqueCount="79">
   <si>
     <t xml:space="preserve">Semana</t>
   </si>
@@ -246,6 +246,18 @@
   <si>
     <t xml:space="preserve">2021-02-25</t>
   </si>
+  <si>
+    <t xml:space="preserve">2021-03-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03-25</t>
+  </si>
 </sst>
 </file>
 
@@ -382,13 +394,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:E1027"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A869" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E875" activeCellId="0" sqref="E875:E951"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A944" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E951" activeCellId="0" sqref="E951:E1027"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
@@ -16564,55 +16576,1298 @@
         <v>43</v>
       </c>
     </row>
-    <row r="952" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="953" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="954" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="955" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="956" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="957" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="958" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="959" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="960" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="961" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="962" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="963" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="964" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="965" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="966" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="967" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="968" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="969" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="970" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="971" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="972" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="973" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="974" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="975" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="976" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="977" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="978" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="979" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="980" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="981" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="982" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="983" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="984" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="985" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="986" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A952" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B952" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C952" s="1" t="n">
+        <v>5426</v>
+      </c>
+      <c r="D952" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="E952" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="953" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A953" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B953" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C953" s="1" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D953" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E953" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="954" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A954" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B954" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C954" s="1" t="n">
+        <v>961</v>
+      </c>
+      <c r="D954" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E954" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="955" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A955" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B955" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C955" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="D955" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E955" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="956" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A956" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B956" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C956" s="1" t="n">
+        <v>1674</v>
+      </c>
+      <c r="D956" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E956" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="957" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A957" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B957" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C957" s="1" t="n">
+        <v>1160</v>
+      </c>
+      <c r="D957" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E957" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="958" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A958" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B958" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C958" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="D958" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E958" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="959" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A959" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B959" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C959" s="1" t="n">
+        <v>991</v>
+      </c>
+      <c r="D959" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E959" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="960" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A960" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B960" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C960" s="1" t="n">
+        <v>1535</v>
+      </c>
+      <c r="D960" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="E960" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="961" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A961" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B961" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C961" s="1" t="n">
+        <v>7627</v>
+      </c>
+      <c r="D961" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="E961" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="962" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A962" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B962" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C962" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="D962" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E962" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="963" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A963" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B963" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C963" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="D963" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E963" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="964" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A964" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B964" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C964" s="1" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D964" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E964" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="965" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A965" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B965" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C965" s="1" t="n">
+        <v>2130</v>
+      </c>
+      <c r="D965" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E965" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="966" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A966" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B966" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C966" s="1" t="n">
+        <v>7864</v>
+      </c>
+      <c r="D966" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="E966" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="967" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A967" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B967" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C967" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="D967" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E967" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="968" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A968" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B968" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C968" s="1" t="n">
+        <v>566</v>
+      </c>
+      <c r="D968" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E968" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="969" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A969" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B969" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C969" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="D969" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E969" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="970" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A970" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B970" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C970" s="1" t="n">
+        <v>2047</v>
+      </c>
+      <c r="D970" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="E970" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="971" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A971" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B971" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C971" s="1" t="n">
+        <v>5810</v>
+      </c>
+      <c r="D971" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="E971" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="972" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A972" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B972" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C972" s="1" t="n">
+        <v>866</v>
+      </c>
+      <c r="D972" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E972" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="973" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A973" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B973" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C973" s="1" t="n">
+        <v>868</v>
+      </c>
+      <c r="D973" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E973" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="974" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A974" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B974" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C974" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="D974" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E974" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="975" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A975" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B975" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C975" s="1" t="n">
+        <v>1724</v>
+      </c>
+      <c r="D975" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E975" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="976" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A976" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B976" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C976" s="1" t="n">
+        <v>1336</v>
+      </c>
+      <c r="D976" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E976" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="977" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A977" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B977" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C977" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="D977" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E977" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="978" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A978" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B978" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C978" s="1" t="n">
+        <v>853</v>
+      </c>
+      <c r="D978" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E978" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="979" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A979" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B979" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C979" s="1" t="n">
+        <v>1272</v>
+      </c>
+      <c r="D979" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="E979" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="980" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A980" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B980" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C980" s="1" t="n">
+        <v>6605</v>
+      </c>
+      <c r="D980" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E980" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="981" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A981" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B981" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C981" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="D981" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E981" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="982" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A982" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B982" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C982" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="D982" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E982" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="983" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A983" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B983" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C983" s="1" t="n">
+        <v>1036</v>
+      </c>
+      <c r="D983" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E983" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="984" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A984" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B984" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C984" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="D984" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E984" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="985" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A985" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B985" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C985" s="1" t="n">
+        <v>7522</v>
+      </c>
+      <c r="D985" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="E985" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="986" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A986" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B986" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C986" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="D986" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E986" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="987" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A987" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B987" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C987" s="1" t="n">
+        <v>533</v>
+      </c>
+      <c r="D987" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E987" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="988" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A988" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B988" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C988" s="1" t="n">
+        <v>435</v>
+      </c>
+      <c r="D988" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E988" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="989" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A989" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B989" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C989" s="1" t="n">
+        <v>1876</v>
+      </c>
+      <c r="D989" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E989" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="990" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A990" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B990" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C990" s="1" t="n">
+        <v>5360</v>
+      </c>
+      <c r="D990" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="E990" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="991" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A991" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B991" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C991" s="1" t="n">
+        <v>791</v>
+      </c>
+      <c r="D991" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E991" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="992" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A992" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B992" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C992" s="1" t="n">
+        <v>892</v>
+      </c>
+      <c r="D992" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E992" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A993" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B993" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C993" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="D993" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E993" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A994" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B994" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C994" s="1" t="n">
+        <v>865</v>
+      </c>
+      <c r="D994" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E994" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A995" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B995" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C995" s="1" t="n">
+        <v>1479</v>
+      </c>
+      <c r="D995" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E995" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A996" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B996" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C996" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="D996" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E996" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="997" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A997" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B997" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C997" s="1" t="n">
+        <v>850</v>
+      </c>
+      <c r="D997" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E997" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A998" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B998" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C998" s="1" t="n">
+        <v>1338</v>
+      </c>
+      <c r="D998" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E998" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A999" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B999" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C999" s="1" t="n">
+        <v>7146</v>
+      </c>
+      <c r="D999" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E999" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1000" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1000" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1000" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="D1000" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1000" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1001" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1001" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1001" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1001" s="1" t="n">
+        <v>540</v>
+      </c>
+      <c r="D1001" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1001" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1002" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1002" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1002" s="1" t="n">
+        <v>1101</v>
+      </c>
+      <c r="D1002" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E1002" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1003" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1003" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1003" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="D1003" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1003" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1004" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1004" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1004" s="1" t="n">
+        <v>7943</v>
+      </c>
+      <c r="D1004" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="E1004" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1005" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1005" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1005" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="D1005" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1005" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1006" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1006" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1006" s="1" t="n">
+        <v>419</v>
+      </c>
+      <c r="D1006" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1006" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1007" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1007" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1007" s="1" t="n">
+        <v>466</v>
+      </c>
+      <c r="D1007" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1007" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1008" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1008" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1008" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1008" s="1" t="n">
+        <v>2092</v>
+      </c>
+      <c r="D1008" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E1008" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1009" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1009" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1009" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1009" s="1" t="n">
+        <v>5992</v>
+      </c>
+      <c r="D1009" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="E1009" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1010" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1010" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1010" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1010" s="1" t="n">
+        <v>956</v>
+      </c>
+      <c r="D1010" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E1010" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1011" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1011" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1011" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1011" s="1" t="n">
+        <v>757</v>
+      </c>
+      <c r="D1011" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E1011" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1012" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1012" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1012" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1012" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="D1012" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1012" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1013" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1013" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1013" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1013" s="1" t="n">
+        <v>721</v>
+      </c>
+      <c r="D1013" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E1013" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1014" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1014" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1014" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1014" s="1" t="n">
+        <v>1547</v>
+      </c>
+      <c r="D1014" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E1014" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1015" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1015" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1015" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1015" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="D1015" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1015" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1016" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1016" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1016" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1016" s="1" t="n">
+        <v>1041</v>
+      </c>
+      <c r="D1016" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E1016" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1017" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1017" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1017" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1017" s="1" t="n">
+        <v>1386</v>
+      </c>
+      <c r="D1017" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="E1017" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1018" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1018" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1018" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1018" s="1" t="n">
+        <v>8227</v>
+      </c>
+      <c r="D1018" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E1018" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1019" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1019" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1019" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1019" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D1019" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1019" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1020" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1020" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1020" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1020" s="1" t="n">
+        <v>479</v>
+      </c>
+      <c r="D1020" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1020" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1021" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1021" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1021" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1021" s="1" t="n">
+        <v>960</v>
+      </c>
+      <c r="D1021" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E1021" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1022" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1022" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1022" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1022" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="D1022" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1022" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1023" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1023" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1023" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1023" s="1" t="n">
+        <v>8353</v>
+      </c>
+      <c r="D1023" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="E1023" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1024" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1024" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1024" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1024" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="D1024" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1024" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1025" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1025" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1025" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1025" s="1" t="n">
+        <v>430</v>
+      </c>
+      <c r="D1025" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E1025" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1026" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1026" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1026" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1026" s="1" t="n">
+        <v>861</v>
+      </c>
+      <c r="D1026" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1026" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1027" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1027" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1027" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1027" s="1" t="n">
+        <v>2481</v>
+      </c>
+      <c r="D1027" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1027" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>